<commit_message>
edit link refs in surv123 tables
</commit_message>
<xml_diff>
--- a/tables/Survey123_app_criteria2.xlsx
+++ b/tables/Survey123_app_criteria2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-deviceIEP\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B17A518-5D68-485A-A471-D736215594EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11AF1E46-8D2D-4BBF-A13A-6341ACD422DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29460" yWindow="795" windowWidth="27960" windowHeight="11385" activeTab="5" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms_Options" sheetId="1" r:id="rId1"/>
@@ -495,10 +495,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Uses device navigation: phone app or GPS device; Data can open in data in ArcGIS maps directly; Can change base map; Default is current location; Can tap the map to change location [test](https://doc.arcgis.com/en/survey123/browser/analyze-results/viewresults.htm#:~:text=Under%20the%20title%20for%20your,geodatabase%20and%20download%20your%20data)
-</t>
-  </si>
-  <si>
     <t>Web Designer</t>
   </si>
   <si>
@@ -529,9 +525,6 @@
   </si>
   <si>
     <t>This can be done with Web Designer using the ‘Set rule function’; However, in Web Designer, this function is limited to Single choice, Dropdown, Likert scale, and Rating questions</t>
-  </si>
-  <si>
-    <t>[tst4](https://support.esri.com/en/technical-article/000022942)</t>
   </si>
   <si>
     <t>External</t>
@@ -828,6 +821,13 @@
   </si>
   <si>
     <t>In trial demo: User noted that it was not possible to view the full list of fish lengths, and it was not easy to edit responses ‘on-the-fly’) [See Yolo BiPass Survey123 Demo](#yoldem))</t>
+  </si>
+  <si>
+    <t>[esri_techsupport](https://support.esri.com/en/technical-article/000022942)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uses device navigation: phone app or GPS device; Data can open in data in ArcGIS maps directly; Can change base map; Default is current location; Can tap the map to change location [arcgis_techsupport](https://doc.arcgis.com/en/survey123/browser/analyze-results/viewresults.htm#:~:text=Under%20the%20title%20for%20your,geodatabase%20and%20download%20your%20data)
+</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEDC525-B77D-4397-8B91-1C5526620A5B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="105" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,10 +1405,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1425,7 +1425,7 @@
         <v>64</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1439,10 +1439,10 @@
         <v>63</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1456,10 +1456,10 @@
         <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1473,13 +1473,13 @@
         <v>63</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1493,7 +1493,7 @@
         <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1523,10 +1523,10 @@
         <v>63</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1537,13 +1537,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>77</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,16 +1565,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1582,16 +1582,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1602,13 +1602,13 @@
         <v>4</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F14" s="18"/>
     </row>
@@ -1623,13 +1623,13 @@
         <v>63</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1643,13 +1643,13 @@
         <v>63</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1674,10 +1674,10 @@
         <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1691,10 +1691,10 @@
         <v>63</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1733,10 +1733,10 @@
         <v>63</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -1750,7 +1750,7 @@
         <v>63</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1802,10 +1802,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1813,17 +1813,17 @@
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>63</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1834,13 +1834,13 @@
         <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F3" s="9"/>
     </row>
@@ -1849,16 +1849,16 @@
         <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1869,13 +1869,13 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F5" s="4"/>
     </row>
@@ -1890,11 +1890,11 @@
         <v>63</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1905,16 +1905,16 @@
         <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="F7" s="8" t="s">
         <v>102</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="G7" s="5"/>
     </row>
@@ -1929,7 +1929,7 @@
         <v>63</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1954,10 +1954,10 @@
         <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1992,10 +1992,10 @@
         <v>62</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2009,7 +2009,7 @@
         <v>63</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="5" customFormat="1" ht="254.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2023,7 +2023,7 @@
         <v>63</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
         <v>63</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2051,10 +2051,10 @@
         <v>63</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -2068,10 +2068,10 @@
         <v>63</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2085,7 +2085,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="93" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2096,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2135,10 +2135,10 @@
         <v>58</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2178,7 +2178,7 @@
         <v>63</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
@@ -2194,7 +2194,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2231,10 +2231,10 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2243,10 +2243,10 @@
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2257,10 +2257,10 @@
         <v>63</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2280,7 +2280,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2289,10 +2289,10 @@
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2304,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DAF0C1-5840-4498-93BE-7596EB0B3995}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,13 +2325,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
@@ -2341,10 +2341,10 @@
         <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -2356,10 +2356,10 @@
         <v>52</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -2371,10 +2371,10 @@
         <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2386,7 +2386,7 @@
         <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -2399,7 +2399,7 @@
         <v>53</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -2412,12 +2412,12 @@
         <v>54</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>

</xml_diff>